<commit_message>
added Datim orgunits ids for Gaza
</commit_message>
<xml_diff>
--- a/conf/paramConfig.xlsx
+++ b/conf/paramConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asamuel/Projects/ccs-datim-data-import/conf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0046E419-901F-D245-A90F-6E6D171D7B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4548478A-C2D7-1544-A85F-9B3C1F83913D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19540" activeTab="7" xr2:uid="{4E933D9A-35E3-C745-AC08-A164B8EEBD08}"/>
+    <workbookView xWindow="15400" yWindow="500" windowWidth="26800" windowHeight="19560" firstSheet="2" activeTab="9" xr2:uid="{4E933D9A-35E3-C745-AC08-A164B8EEBD08}"/>
   </bookViews>
   <sheets>
     <sheet name="mer_datasets_id" sheetId="7" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="396">
   <si>
     <t>MER C&amp;T</t>
   </si>
@@ -473,12 +473,6 @@
     <t>Romao</t>
   </si>
   <si>
-    <t>Pcanico</t>
-  </si>
-  <si>
-    <t>Ccivil</t>
-  </si>
-  <si>
     <t>Malhangalene</t>
   </si>
   <si>
@@ -488,15 +482,9 @@
     <t>Maxaquene</t>
   </si>
   <si>
-    <t>Pcimento</t>
-  </si>
-  <si>
     <t>HPI</t>
   </si>
   <si>
-    <t>Mtendas</t>
-  </si>
-  <si>
     <t>Incassane</t>
   </si>
   <si>
@@ -1154,9 +1142,6 @@
     <t>DSD PREP,DSD TB PREV,DSD GEND GBV,DSD FPINT SITE</t>
   </si>
   <si>
-    <t>DSD HTS TST COMMUNITY OTHER,DSD HTS INDEX COMMUNITY</t>
-  </si>
-  <si>
     <t>LAB PTCQI,PMTCT FO</t>
   </si>
   <si>
@@ -1164,13 +1149,97 @@
   </si>
   <si>
     <t>DSD TX NEW,DSD TX CURR,DSD TX RTT,DSD TX ML,DSD PMCT ART,DSD TX PVLS,DSD TX TB,DSD TB ART</t>
+  </si>
+  <si>
+    <t>yEJF0gLWJ3M</t>
+  </si>
+  <si>
+    <t>foPEfoFVknQ</t>
+  </si>
+  <si>
+    <t>kllBvMTCXLE</t>
+  </si>
+  <si>
+    <t>ydlqLc8aswr</t>
+  </si>
+  <si>
+    <t>QGkcBfi9Y4T</t>
+  </si>
+  <si>
+    <t>GZM6MBIwrs3</t>
+  </si>
+  <si>
+    <t>aH9Lc042Zmu</t>
+  </si>
+  <si>
+    <t>GrEI5LZLmJJ</t>
+  </si>
+  <si>
+    <t>mh2WLX4g3WD</t>
+  </si>
+  <si>
+    <t>ZoR8klcQ1J8</t>
+  </si>
+  <si>
+    <t>Bilene_D</t>
+  </si>
+  <si>
+    <t>Chibuto_D</t>
+  </si>
+  <si>
+    <t>Chokwe_D</t>
+  </si>
+  <si>
+    <t>Chongoene_D</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> XaiXai_D</t>
+  </si>
+  <si>
+    <t>Guija_D</t>
+  </si>
+  <si>
+    <t>Limpopo_D</t>
+  </si>
+  <si>
+    <t>Mabalane_D</t>
+  </si>
+  <si>
+    <t>Mandlakaze_D</t>
+  </si>
+  <si>
+    <t>Mapai_D</t>
+  </si>
+  <si>
+    <t>Massingir_D</t>
+  </si>
+  <si>
+    <t>Qeubs8yLwuO</t>
+  </si>
+  <si>
+    <t>GqENHaHYzP0</t>
+  </si>
+  <si>
+    <t>DSD HTS TST COMMUNITY OTHER,DSD HTS INDEX COMMUNITY,DSD HTS TST COMMUNITY MOBILE</t>
+  </si>
+  <si>
+    <t>PCanico</t>
+  </si>
+  <si>
+    <t>CCivil</t>
+  </si>
+  <si>
+    <t>PCimento</t>
+  </si>
+  <si>
+    <t>MTendas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1181,13 +1250,33 @@
     <font>
       <sz val="12"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF171C1F"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF171C1F"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1210,17 +1299,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1567,21 +1679,21 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B1" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1589,7 +1701,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1597,7 +1709,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1605,7 +1717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1613,7 +1725,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1621,7 +1733,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1629,7 +1741,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1637,7 +1749,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1652,829 +1764,930 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1C226DE-F020-454C-975D-64191FC04A0B}">
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="21.5" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="B1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C57" s="3"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="C61" s="3"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C66" s="3"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="B103" s="7" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B14" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>185</v>
-      </c>
-      <c r="B15" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>187</v>
-      </c>
-      <c r="B16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>189</v>
-      </c>
-      <c r="B17" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>191</v>
-      </c>
-      <c r="B18" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>193</v>
-      </c>
-      <c r="B19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>195</v>
-      </c>
-      <c r="B20" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>197</v>
-      </c>
-      <c r="B21" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>199</v>
-      </c>
-      <c r="B22" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>201</v>
-      </c>
-      <c r="B23" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>203</v>
-      </c>
-      <c r="B24" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>205</v>
-      </c>
-      <c r="B25" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>207</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B104" s="7" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>209</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B105" s="7" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>211</v>
-      </c>
-      <c r="B28" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>213</v>
-      </c>
-      <c r="B29" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>215</v>
-      </c>
-      <c r="B30" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>217</v>
-      </c>
-      <c r="B31" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>219</v>
-      </c>
-      <c r="B32" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>221</v>
-      </c>
-      <c r="B33" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>223</v>
-      </c>
-      <c r="B34" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
-        <v>225</v>
-      </c>
-      <c r="B35" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
-        <v>227</v>
-      </c>
-      <c r="B36" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s">
-        <v>229</v>
-      </c>
-      <c r="B37" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
-        <v>231</v>
-      </c>
-      <c r="B38" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
-        <v>233</v>
-      </c>
-      <c r="B39" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
-        <v>235</v>
-      </c>
-      <c r="B40" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" t="s">
-        <v>237</v>
-      </c>
-      <c r="B41" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" t="s">
-        <v>239</v>
-      </c>
-      <c r="B42" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" t="s">
-        <v>241</v>
-      </c>
-      <c r="B43" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" t="s">
-        <v>243</v>
-      </c>
-      <c r="B44" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" t="s">
-        <v>245</v>
-      </c>
-      <c r="B45" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" t="s">
-        <v>247</v>
-      </c>
-      <c r="B46" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" t="s">
-        <v>249</v>
-      </c>
-      <c r="B47" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" t="s">
-        <v>251</v>
-      </c>
-      <c r="B48" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" t="s">
-        <v>253</v>
-      </c>
-      <c r="B49" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" t="s">
-        <v>255</v>
-      </c>
-      <c r="B50" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" t="s">
-        <v>257</v>
-      </c>
-      <c r="B51" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" t="s">
-        <v>259</v>
-      </c>
-      <c r="B52" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" t="s">
-        <v>261</v>
-      </c>
-      <c r="B53" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" t="s">
-        <v>263</v>
-      </c>
-      <c r="B54" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" t="s">
-        <v>265</v>
-      </c>
-      <c r="B55" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
-      <c r="A56" t="s">
-        <v>267</v>
-      </c>
-      <c r="B56" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" t="s">
-        <v>269</v>
-      </c>
-      <c r="B57" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" t="s">
-        <v>271</v>
-      </c>
-      <c r="B58" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" t="s">
-        <v>273</v>
-      </c>
-      <c r="B59" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B111" s="7" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="A60" t="s">
-        <v>275</v>
-      </c>
-      <c r="B60" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
-      <c r="A61" t="s">
-        <v>277</v>
-      </c>
-      <c r="B61" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
-      <c r="A62" t="s">
-        <v>279</v>
-      </c>
-      <c r="B62" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
-      <c r="A63" t="s">
-        <v>281</v>
-      </c>
-      <c r="B63" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" t="s">
-        <v>283</v>
-      </c>
-      <c r="B64" t="s">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B112" s="7" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" t="s">
-        <v>285</v>
-      </c>
-      <c r="B65" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
-      <c r="A66" t="s">
-        <v>287</v>
-      </c>
-      <c r="B66" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" t="s">
-        <v>289</v>
-      </c>
-      <c r="B67" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" t="s">
-        <v>291</v>
-      </c>
-      <c r="B68" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" t="s">
-        <v>293</v>
-      </c>
-      <c r="B69" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" t="s">
-        <v>295</v>
-      </c>
-      <c r="B70" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" t="s">
-        <v>297</v>
-      </c>
-      <c r="B71" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" t="s">
-        <v>299</v>
-      </c>
-      <c r="B72" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" t="s">
-        <v>301</v>
-      </c>
-      <c r="B73" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" t="s">
-        <v>303</v>
-      </c>
-      <c r="B74" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" t="s">
-        <v>305</v>
-      </c>
-      <c r="B75" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" t="s">
-        <v>307</v>
-      </c>
-      <c r="B76" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" t="s">
-        <v>309</v>
-      </c>
-      <c r="B77" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" t="s">
-        <v>311</v>
-      </c>
-      <c r="B78" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" t="s">
-        <v>313</v>
-      </c>
-      <c r="B79" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80" t="s">
-        <v>315</v>
-      </c>
-      <c r="B80" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" t="s">
-        <v>317</v>
-      </c>
-      <c r="B81" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" t="s">
-        <v>319</v>
-      </c>
-      <c r="B82" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" t="s">
-        <v>321</v>
-      </c>
-      <c r="B83" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" t="s">
-        <v>323</v>
-      </c>
-      <c r="B84" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" t="s">
-        <v>325</v>
-      </c>
-      <c r="B85" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" t="s">
-        <v>327</v>
-      </c>
-      <c r="B86" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" t="s">
-        <v>329</v>
-      </c>
-      <c r="B87" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88" t="s">
-        <v>331</v>
-      </c>
-      <c r="B88" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" t="s">
-        <v>333</v>
-      </c>
-      <c r="B89" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" t="s">
-        <v>335</v>
-      </c>
-      <c r="B90" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" t="s">
-        <v>337</v>
-      </c>
-      <c r="B91" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" t="s">
-        <v>339</v>
-      </c>
-      <c r="B92" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" t="s">
-        <v>341</v>
-      </c>
-      <c r="B93" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" t="s">
-        <v>343</v>
-      </c>
-      <c r="B94" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" t="s">
-        <v>345</v>
-      </c>
-      <c r="B95" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" t="s">
-        <v>347</v>
-      </c>
-      <c r="B96" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
-      <c r="A97" t="s">
-        <v>349</v>
-      </c>
-      <c r="B97" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
-      <c r="A98" t="s">
-        <v>350</v>
-      </c>
-      <c r="B98" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
-      <c r="A99" t="s">
-        <v>352</v>
-      </c>
-      <c r="B99" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
-      <c r="A100" t="s">
-        <v>354</v>
-      </c>
-      <c r="B100" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2">
-      <c r="A101" t="s">
-        <v>356</v>
-      </c>
-      <c r="B101" t="s">
-        <v>357</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B101">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B28 B30:B60 B62:B101">
+    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30:B60 B1:B28 B62:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2488,21 +2701,21 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2510,7 +2723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2518,7 +2731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2526,7 +2739,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2534,7 +2747,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2542,7 +2755,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2550,7 +2763,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2571,21 +2784,21 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B1" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2593,7 +2806,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2601,7 +2814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2609,7 +2822,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2617,7 +2830,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2625,7 +2838,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2633,7 +2846,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2641,7 +2854,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2662,21 +2875,21 @@
       <selection activeCell="B1" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -2684,7 +2897,7 @@
         <v>202409</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
@@ -2692,7 +2905,7 @@
         <v>202410</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
@@ -2700,7 +2913,7 @@
         <v>202411</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -2708,7 +2921,7 @@
         <v>202412</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -2716,7 +2929,7 @@
         <v>202501</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -2724,7 +2937,7 @@
         <v>202502</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
@@ -2732,7 +2945,7 @@
         <v>202503</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
@@ -2740,7 +2953,7 @@
         <v>202504</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
@@ -2748,7 +2961,7 @@
         <v>202505</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -2756,7 +2969,7 @@
         <v>202506</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -2764,7 +2977,7 @@
         <v>202507</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -2772,7 +2985,7 @@
         <v>202508</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
@@ -2780,7 +2993,7 @@
         <v>202509</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
@@ -2788,7 +3001,7 @@
         <v>202510</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>45</v>
       </c>
@@ -2796,7 +3009,7 @@
         <v>202511</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
@@ -2817,21 +3030,21 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.5" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -2839,7 +3052,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -2847,7 +3060,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2855,7 +3068,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2863,7 +3076,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -2871,7 +3084,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -2879,7 +3092,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -2887,7 +3100,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -2908,20 +3121,20 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B1" t="s">
         <v>358</v>
       </c>
-      <c r="B1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -2942,21 +3155,21 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B1" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -2964,7 +3177,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -2972,7 +3185,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -2980,7 +3193,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -2988,7 +3201,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -2996,7 +3209,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -3004,7 +3217,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -3021,78 +3234,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{617E2EE4-4FAE-904B-B397-EE44A2034DC2}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="91.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="B2" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="B3" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="B4" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="B5" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="B6" s="2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="B7" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>84</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>371</v>
+      <c r="B8" s="2" t="s">
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -3106,316 +3319,316 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="21.5" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="B1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="B7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="2" t="s">
+      <c r="B19" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="B15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="2" t="s">
+      <c r="B26" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="B16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="2" t="s">
+      <c r="B27" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="B19" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B20" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B21" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="2" t="s">
+      <c r="B30" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B22" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B23" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B24" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B25" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="2" t="s">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B26" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B27" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B28" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B29" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B30" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B31" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B32" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B33" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="2" t="s">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="2" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="2" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="2" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="2" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>136</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix Marien Ngoabi e Chocke HR datim codeds
</commit_message>
<xml_diff>
--- a/conf/paramConfig.xlsx
+++ b/conf/paramConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asamuel/Projects/ccs-datim-data-import/conf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4548478A-C2D7-1544-A85F-9B3C1F83913D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA61108-590D-0241-BFCD-41B5CDDE88FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15400" yWindow="500" windowWidth="26800" windowHeight="19560" firstSheet="2" activeTab="9" xr2:uid="{4E933D9A-35E3-C745-AC08-A164B8EEBD08}"/>
+    <workbookView xWindow="1880" yWindow="500" windowWidth="36520" windowHeight="19560" activeTab="5" xr2:uid="{4E933D9A-35E3-C745-AC08-A164B8EEBD08}"/>
   </bookViews>
   <sheets>
     <sheet name="mer_datasets_id" sheetId="7" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="399">
   <si>
     <t>MER C&amp;T</t>
   </si>
@@ -236,9 +236,6 @@
     <t>2025Q4</t>
   </si>
   <si>
-    <t>funding_mechanism</t>
-  </si>
-  <si>
     <t>excell_mapping_template_mer_ct</t>
   </si>
   <si>
@@ -1233,13 +1230,25 @@
   </si>
   <si>
     <t>MTendas</t>
+  </si>
+  <si>
+    <t>kZka73xT1AZ</t>
+  </si>
+  <si>
+    <t>funding_mechanism_maputo</t>
+  </si>
+  <si>
+    <t>funding_mechanism_gaza</t>
+  </si>
+  <si>
+    <t>Chokwe_HR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1277,6 +1286,13 @@
       <sz val="13"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1299,7 +1315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1308,6 +1324,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1687,10 +1704,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1764,929 +1781,938 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1C226DE-F020-454C-975D-64191FC04A0B}">
-  <dimension ref="A1:C112"/>
+  <dimension ref="A1:C113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>376</v>
-      </c>
-      <c r="C29" s="3"/>
+        <v>398</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>212</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C45" s="3"/>
+        <v>239</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>244</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="C46" s="3"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="C57" s="3"/>
+        <v>263</v>
+      </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>268</v>
-      </c>
+        <v>265</v>
+      </c>
+      <c r="C58" s="3"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>377</v>
-      </c>
-      <c r="C61" s="3"/>
+        <v>270</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>276</v>
-      </c>
+        <v>272</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="C62" s="3"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>282</v>
-      </c>
+      <c r="C65" s="8"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="C66" s="3"/>
+        <v>281</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>286</v>
-      </c>
+        <v>388</v>
+      </c>
+      <c r="C67" s="3"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>374</v>
+        <v>341</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>344</v>
+        <v>373</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B102" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" s="4" t="s">
-        <v>378</v>
-      </c>
-      <c r="B102" s="7" t="s">
-        <v>368</v>
-      </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" s="1" t="s">
-        <v>379</v>
+      <c r="A103" s="4" t="s">
+        <v>377</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>182</v>
+        <v>367</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>369</v>
+        <v>209</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>274</v>
+        <v>372</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>284</v>
+        <v>273</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B28 B30:B60 B62:B101">
+  <conditionalFormatting sqref="B2:B29 B31:B61 B63:B102">
     <cfRule type="duplicateValues" dxfId="1" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30:B60 B1:B28 B62:B1048576">
+  <conditionalFormatting sqref="B31:B61 B1:B29 B63:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2709,10 +2735,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B1" t="s">
         <v>354</v>
-      </c>
-      <c r="B1" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2792,10 +2818,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2883,10 +2909,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B1" t="s">
         <v>357</v>
-      </c>
-      <c r="B1" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -3038,10 +3064,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B1" t="s">
         <v>357</v>
-      </c>
-      <c r="B1" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -3115,31 +3141,39 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{849AD34E-7686-0A42-93B7-B225DA2E3DAB}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>396</v>
       </c>
       <c r="B2">
         <v>160451</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B3">
+        <v>81776</v>
       </c>
     </row>
   </sheetData>
@@ -3163,66 +3197,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -3246,66 +3280,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -3330,306 +3364,306 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug Fix: PMTCT_HEI_POS_ART Wrong DE Mapping
</commit_message>
<xml_diff>
--- a/conf/paramConfig.xlsx
+++ b/conf/paramConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asamuel/Projects/ccs-datim-data-import/conf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F00AAE6-74F1-F04C-AADF-339551562D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421B31C1-6F42-BF43-B4C8-A69E85B094E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="1620" windowWidth="36400" windowHeight="17320" firstSheet="1" activeTab="10" xr2:uid="{4E933D9A-35E3-C745-AC08-A164B8EEBD08}"/>
+    <workbookView xWindow="6140" yWindow="2680" windowWidth="36400" windowHeight="17320" activeTab="6" xr2:uid="{4E933D9A-35E3-C745-AC08-A164B8EEBD08}"/>
   </bookViews>
   <sheets>
     <sheet name="ccs_datim_exchange_orgunits" sheetId="13" r:id="rId1"/>
@@ -11964,7 +11964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1C226DE-F020-454C-975D-64191FC04A0B}">
   <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+    <sheetView topLeftCell="A80" workbookViewId="0">
       <selection activeCell="J106" sqref="J106"/>
     </sheetView>
   </sheetViews>
@@ -13439,8 +13439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{849AD34E-7686-0A42-93B7-B225DA2E3DAB}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13461,7 +13461,7 @@
         <v>396</v>
       </c>
       <c r="B2">
-        <v>160451</v>
+        <v>81776</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -13474,6 +13474,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>